<commit_message>
Planilha de Riscos feita
</commit_message>
<xml_diff>
--- a/Matriz de Risco/5_MatrizRisco_Template.xlsx
+++ b/Matriz de Risco/5_MatrizRisco_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Rosilene\Documents\Trabalho\PUC\BES\Aulas 2023_2\BES_GesPortifólio\Aulas\Artefatos - GPP_TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gestao-de-Portfolios\Matriz de Risco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15F0195-ED0B-4C60-8E09-36EB4A889DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE7B5CE-F781-4CC0-B613-BD43E1939B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{61E249DC-A331-4BE8-BBA5-8E40E4D212F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{61E249DC-A331-4BE8-BBA5-8E40E4D212F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de Riscos" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>RISCOS IDENTIFICADOS</t>
   </si>
@@ -85,6 +85,81 @@
   </si>
   <si>
     <t>SEVERIDADE</t>
+  </si>
+  <si>
+    <t>Atrasos no desenvolvimento da Plataforma de Automação de Testes de Software</t>
+  </si>
+  <si>
+    <t>O atraso pode comprometer a eficiência das equipes de desenvolvimento e reduzir a competitividade no mercado.</t>
+  </si>
+  <si>
+    <t>Mitigar</t>
+  </si>
+  <si>
+    <t>Implementar metodologias ágeis e monitoramento frequente dos prazos</t>
+  </si>
+  <si>
+    <t>Baixa adesão à Plataforma de Treinamento para Equipes de Desenvolvimento</t>
+  </si>
+  <si>
+    <t>As equipes podem não utilizar adequadamente, resultando em baixo ROI.</t>
+  </si>
+  <si>
+    <t>Programa de capacitação e incentivo para o uso da plataforma</t>
+  </si>
+  <si>
+    <t>Mudanças frequentes podem gerar retrabalho, custos e prazos aumentados.</t>
+  </si>
+  <si>
+    <t>Definir escopo claro e processos robustos de gerenciamento de mudanças</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Mudanças constantes nos requisitos da Plataforma de Gestão de Requisitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Falta de inovação no Projeto de Pesquisa e Melhoria Contínua dos Processos</t>
+  </si>
+  <si>
+    <t>Falta de melhorias pode resultar na perda de competitividade e estagnação.</t>
+  </si>
+  <si>
+    <t>Investir em pesquisa contínua e parcerias com universidades ou startups</t>
+  </si>
+  <si>
+    <t>Falha de integração com sistemas legados no Laboratório de Inovação para Engenharia de Software</t>
+  </si>
+  <si>
+    <t>A incompatibilidade tecnológica pode atrasar a implementação e causar custos adicionais.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Planejar fases de teste rigorosas e utilização de APIs bem documentadas</t>
+  </si>
+  <si>
+    <t>Sobrecarga de recursos em múltiplos projetos simultâneos</t>
+  </si>
+  <si>
+    <t>A equipe pode ficar sobrecarregada, resultando em atrasos e baixa qualidade.</t>
+  </si>
+  <si>
+    <t>Alocar recursos com base na prioridade e monitorar a carga de trabalho</t>
+  </si>
+  <si>
+    <t>Falta de feedback contínuo para o Projeto de Pesquisa e Melhoria Contínua dos Processos</t>
+  </si>
+  <si>
+    <t>Sem feedback adequado, as melhorias podem ser mal direcionadas.</t>
+  </si>
+  <si>
+    <t>Implementar ciclos curtos de feedback com stakeholders e usuários</t>
+  </si>
+  <si>
+    <t>Custos elevados no desenvolvimento da Plataforma de Gestão de Requisitos</t>
+  </si>
+  <si>
+    <t>O aumento nos custos pode comprometer o ROI e a viabilidade do projeto.</t>
+  </si>
+  <si>
+    <t>Acompanhamento contínuo do orçamento e revisão das funcionalidades</t>
   </si>
 </sst>
 </file>
@@ -509,128 +584,128 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1001,9 +1076,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1041,7 +1116,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1147,7 +1222,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1289,7 +1364,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1305,249 +1380,361 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F7" sqref="F7"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="2.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="49" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="20" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="20" t="s">
+      <c r="F2" s="60"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="21"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="I2" s="57"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="42"/>
-      <c r="C4" s="56">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="24"/>
-    </row>
-    <row r="5" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="43"/>
-      <c r="C5" s="57">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="24"/>
-    </row>
-    <row r="6" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="56">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="24"/>
-    </row>
-    <row r="7" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
-      <c r="C7" s="57">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="24"/>
-    </row>
-    <row r="8" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="42"/>
-      <c r="C8" s="56">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="24"/>
-    </row>
-    <row r="9" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="57">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="56">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="24"/>
-    </row>
-    <row r="11" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="57">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="58">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="26"/>
+    <row r="4" spans="2:9" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="39">
+        <v>1</v>
+      </c>
+      <c r="C4" s="51">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>6</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="24">
+        <v>2</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="40">
+        <v>2</v>
+      </c>
+      <c r="C5" s="52">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>4</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="24">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="39">
+        <v>3</v>
+      </c>
+      <c r="C6" s="51">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>6</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="24">
+        <v>3</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="40">
+        <v>4</v>
+      </c>
+      <c r="C7" s="52">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="24">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>3</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="39">
+        <v>5</v>
+      </c>
+      <c r="C8" s="51">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>4</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="24">
+        <v>2</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="40">
+        <v>6</v>
+      </c>
+      <c r="C9" s="52">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>6</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="24">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10">
+        <v>3</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="39">
+        <v>7</v>
+      </c>
+      <c r="C10" s="51">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>2</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="24">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="40">
+        <v>8</v>
+      </c>
+      <c r="C11" s="52">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>4</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="24">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="41"/>
+      <c r="C12" s="53">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
-      <c r="C13" s="59">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="26"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="2:9" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="42"/>
+      <c r="C13" s="54">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="49"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="24"/>
-    </row>
-    <row r="14" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="44"/>
-      <c r="C14" s="58">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="26"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="2:9" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="41"/>
+      <c r="C14" s="53">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="24"/>
-    </row>
-    <row r="15" spans="2:9" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="45"/>
-      <c r="C15" s="59">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="26"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="2:9" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="42"/>
+      <c r="C15" s="54">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="48"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="24"/>
-    </row>
-    <row r="16" spans="2:9" s="16" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="46"/>
-      <c r="C16" s="60">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="29"/>
-      <c r="C17" s="29">
-        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="30"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="2:9" s="16" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="43"/>
+      <c r="C16" s="55">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="50"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="27"/>
+      <c r="C17" s="27">
+        <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12"/>
       <c r="C18" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1560,7 +1747,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14"/>
       <c r="C19" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1573,7 +1760,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1586,7 +1773,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14"/>
       <c r="C21" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1599,7 +1786,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" s="12"/>
       <c r="C22" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1612,7 +1799,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B23" s="14"/>
       <c r="C23" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1625,7 +1812,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
       <c r="C24" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1638,7 +1825,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="C25" s="6">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1651,7 +1838,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
       <c r="C26" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1664,7 +1851,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14"/>
       <c r="C27" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1677,7 +1864,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12"/>
       <c r="C28" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1690,7 +1877,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B29" s="14"/>
       <c r="C29" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1703,7 +1890,7 @@
       <c r="H29" s="7"/>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B30" s="12"/>
       <c r="C30" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1716,7 +1903,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14"/>
       <c r="C31" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1729,7 +1916,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" s="12"/>
       <c r="C32" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1742,7 +1929,7 @@
       <c r="H32" s="7"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="14"/>
       <c r="C33" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1755,7 +1942,7 @@
       <c r="H33" s="7"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1768,7 +1955,7 @@
       <c r="H34" s="7"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" s="6"/>
       <c r="C35" s="6">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1781,7 +1968,7 @@
       <c r="H35" s="4"/>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" s="12"/>
       <c r="C36" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1794,7 +1981,7 @@
       <c r="H36" s="7"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14"/>
       <c r="C37" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1807,7 +1994,7 @@
       <c r="H37" s="7"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="C38" s="12">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1820,7 +2007,7 @@
       <c r="H38" s="7"/>
       <c r="I38" s="11"/>
     </row>
-    <row r="39" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" s="14"/>
       <c r="C39" s="14">
         <f>Tabela1310[[#This Row],[IMPACTO]]*Tabela1310[[#This Row],[PROBABILIDADE]]</f>
@@ -1833,7 +2020,7 @@
       <c r="H39" s="7"/>
       <c r="I39" s="11"/>
     </row>
-    <row r="40" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
@@ -1842,7 +2029,7 @@
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C41" s="17" t="s">
         <v>7</v>
       </c>
@@ -1850,7 +2037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C42" s="17" t="s">
         <v>8</v>
       </c>
@@ -1858,7 +2045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C43" s="17" t="s">
         <v>11</v>
       </c>

</xml_diff>